<commit_message>
Re-formatted round 4 forecast Excel file
</commit_message>
<xml_diff>
--- a/2016SuperRugby/Weekly Forecasts/Round_4.xlsx
+++ b/2016SuperRugby/Weekly Forecasts/Round_4.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RugbyPredictifier\RugbyPredictifier\2016SuperRugby\Weekly Forecasts\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Friday" sheetId="1" r:id="rId1"/>
     <sheet name="Saturday" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="42">
   <si>
     <t>Chance of Winning</t>
   </si>
@@ -146,12 +151,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#0%"/>
     <numFmt numFmtId="165" formatCode="#0"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -466,6 +471,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -512,7 +525,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -544,9 +557,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -578,6 +592,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -753,7 +768,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BI24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -761,9 +776,17 @@
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="25.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="1.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="1.26953125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:61">
+    <row r="1" spans="1:61" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
@@ -795,30 +818,30 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:61">
+    <row r="2" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="8">
-        <v>0.2589434</v>
+        <v>0.25894339999999999</v>
       </c>
       <c r="C2" s="8">
-        <v>0.7085318</v>
+        <v>0.70853180000000004</v>
       </c>
       <c r="E2" s="8">
-        <v>0.5570818</v>
+        <v>0.55708179999999996</v>
       </c>
       <c r="F2" s="8">
-        <v>0.4175012</v>
+        <v>0.41750120000000002</v>
       </c>
       <c r="H2" s="8">
-        <v>0.2286526</v>
+        <v>0.22865260000000001</v>
       </c>
       <c r="I2" s="8">
-        <v>0.7509882</v>
-      </c>
-    </row>
-    <row r="3" spans="1:61">
+        <v>0.75098819999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
@@ -826,22 +849,22 @@
         <v>15.4915518</v>
       </c>
       <c r="C3" s="9">
-        <v>24.5729932</v>
+        <v>24.572993199999999</v>
       </c>
       <c r="E3" s="9">
-        <v>26.7979028</v>
+        <v>26.797902799999999</v>
       </c>
       <c r="F3" s="9">
         <v>23.6566282</v>
       </c>
       <c r="H3" s="9">
-        <v>19.7492942</v>
+        <v>19.749294200000001</v>
       </c>
       <c r="I3" s="9">
-        <v>32.7641634</v>
-      </c>
-    </row>
-    <row r="4" spans="1:61">
+        <v>32.764163400000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
@@ -864,7 +887,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:61">
+    <row r="5" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
@@ -887,7 +910,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:61">
+    <row r="6" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>4</v>
       </c>
@@ -910,7 +933,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:61">
+    <row r="7" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>5</v>
       </c>
@@ -933,7 +956,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:61">
+    <row r="8" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>6</v>
       </c>
@@ -956,7 +979,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:61">
+    <row r="9" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>7</v>
       </c>
@@ -979,7 +1002,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:61">
+    <row r="10" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>8</v>
       </c>
@@ -1002,7 +1025,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:61">
+    <row r="11" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>9</v>
       </c>
@@ -1025,7 +1048,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:61">
+    <row r="12" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>10</v>
       </c>
@@ -1048,7 +1071,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:61">
+    <row r="13" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>11</v>
       </c>
@@ -1071,7 +1094,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:61">
+    <row r="14" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>12</v>
       </c>
@@ -1094,7 +1117,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:61">
+    <row r="15" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>13</v>
       </c>
@@ -1117,7 +1140,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:61">
+    <row r="16" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
         <v>14</v>
       </c>
@@ -1140,7 +1163,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>15</v>
       </c>
@@ -1163,7 +1186,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>16</v>
       </c>
@@ -1186,7 +1209,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>17</v>
       </c>
@@ -1209,7 +1232,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
         <v>18</v>
       </c>
@@ -1232,7 +1255,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
         <v>19</v>
       </c>
@@ -1255,7 +1278,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
         <v>20</v>
       </c>
@@ -1278,50 +1301,50 @@
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
         <v>21</v>
       </c>
       <c r="B23" s="8">
-        <v>0.0437342</v>
+        <v>4.3734200000000001E-2</v>
       </c>
       <c r="C23" s="8">
-        <v>0.1277086</v>
+        <v>0.12770860000000001</v>
       </c>
       <c r="E23" s="8">
-        <v>0.1895216</v>
+        <v>0.18952160000000001</v>
       </c>
       <c r="F23" s="8">
-        <v>0.089639</v>
+        <v>8.9638999999999996E-2</v>
       </c>
       <c r="H23" s="8">
-        <v>0.0488692</v>
+        <v>4.8869200000000002E-2</v>
       </c>
       <c r="I23" s="8">
-        <v>0.318792</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
+        <v>0.31879200000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
         <v>22</v>
       </c>
       <c r="B24" s="8">
-        <v>0.168031</v>
+        <v>0.16803100000000001</v>
       </c>
       <c r="C24" s="8">
         <v>0.1202448</v>
       </c>
       <c r="E24" s="8">
-        <v>0.1395436</v>
+        <v>0.13954359999999999</v>
       </c>
       <c r="F24" s="8">
-        <v>0.1531152</v>
+        <v>0.15311520000000001</v>
       </c>
       <c r="H24" s="8">
-        <v>0.135363</v>
+        <v>0.13536300000000001</v>
       </c>
       <c r="I24" s="8">
-        <v>0.0976042</v>
+        <v>9.7604200000000002E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1330,7 +1353,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BI24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1338,9 +1361,23 @@
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="25.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="1.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="1.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="1.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="1.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="1.26953125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.36328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:61">
+    <row r="1" spans="1:61" x14ac:dyDescent="0.35">
       <c r="B1" s="10" t="s">
         <v>30</v>
       </c>
@@ -1399,89 +1436,89 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:61">
+    <row r="2" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="8">
-        <v>0.4657798</v>
+        <v>0.46577980000000002</v>
       </c>
       <c r="C2" s="8">
-        <v>0.5136344</v>
+        <v>0.51363440000000005</v>
       </c>
       <c r="E2" s="8">
-        <v>0.9706734</v>
+        <v>0.97067340000000002</v>
       </c>
       <c r="F2" s="8">
-        <v>0.02568</v>
+        <v>2.5680000000000001E-2</v>
       </c>
       <c r="H2" s="8">
-        <v>0.3311278</v>
+        <v>0.33112780000000003</v>
       </c>
       <c r="I2" s="8">
-        <v>0.6486628</v>
+        <v>0.64866279999999998</v>
       </c>
       <c r="K2" s="8">
-        <v>0.5852106</v>
+        <v>0.58521060000000003</v>
       </c>
       <c r="L2" s="8">
-        <v>0.3926708</v>
+        <v>0.39267079999999999</v>
       </c>
       <c r="N2" s="8">
         <v>0.1991994</v>
       </c>
       <c r="O2" s="8">
-        <v>0.7679642</v>
+        <v>0.76796419999999999</v>
       </c>
       <c r="Q2" s="8">
-        <v>0.3678584</v>
+        <v>0.36785839999999997</v>
       </c>
       <c r="R2" s="8">
-        <v>0.6132752</v>
-      </c>
-    </row>
-    <row r="3" spans="1:61">
+        <v>0.61327520000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="9">
-        <v>30.9920318</v>
+        <v>30.992031799999999</v>
       </c>
       <c r="C3" s="9">
-        <v>32.1312936</v>
+        <v>32.131293599999999</v>
       </c>
       <c r="E3" s="9">
-        <v>49.5188234</v>
+        <v>49.518823400000002</v>
       </c>
       <c r="F3" s="9">
         <v>12.7607964</v>
       </c>
       <c r="H3" s="9">
-        <v>19.8198086</v>
+        <v>19.819808600000002</v>
       </c>
       <c r="I3" s="9">
-        <v>26.0507978</v>
+        <v>26.050797800000002</v>
       </c>
       <c r="K3" s="9">
-        <v>33.4399966</v>
+        <v>33.439996600000001</v>
       </c>
       <c r="L3" s="9">
-        <v>28.2856924</v>
+        <v>28.285692399999999</v>
       </c>
       <c r="N3" s="9">
-        <v>14.6281396</v>
+        <v>14.628139600000001</v>
       </c>
       <c r="O3" s="9">
-        <v>28.0759204</v>
+        <v>28.075920400000001</v>
       </c>
       <c r="Q3" s="9">
-        <v>33.1732724</v>
+        <v>33.173272400000002</v>
       </c>
       <c r="R3" s="9">
-        <v>39.8244768</v>
-      </c>
-    </row>
-    <row r="4" spans="1:61">
+        <v>39.824476799999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
@@ -1522,7 +1559,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:61">
+    <row r="5" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
@@ -1563,7 +1600,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:61">
+    <row r="6" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>4</v>
       </c>
@@ -1604,7 +1641,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:61">
+    <row r="7" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>5</v>
       </c>
@@ -1645,7 +1682,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:61">
+    <row r="8" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>6</v>
       </c>
@@ -1686,7 +1723,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:61">
+    <row r="9" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>7</v>
       </c>
@@ -1727,7 +1764,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:61">
+    <row r="10" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>8</v>
       </c>
@@ -1768,7 +1805,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:61">
+    <row r="11" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>9</v>
       </c>
@@ -1809,7 +1846,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:61">
+    <row r="12" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>10</v>
       </c>
@@ -1850,7 +1887,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:61">
+    <row r="13" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>11</v>
       </c>
@@ -1891,7 +1928,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:61">
+    <row r="14" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>12</v>
       </c>
@@ -1932,7 +1969,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:61">
+    <row r="15" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>13</v>
       </c>
@@ -1973,7 +2010,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:61">
+    <row r="16" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
         <v>14</v>
       </c>
@@ -2014,7 +2051,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>15</v>
       </c>
@@ -2055,7 +2092,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:18">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>16</v>
       </c>
@@ -2096,7 +2133,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:18">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>17</v>
       </c>
@@ -2137,7 +2174,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
         <v>18</v>
       </c>
@@ -2178,7 +2215,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:18">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
         <v>19</v>
       </c>
@@ -2219,7 +2256,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:18">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
         <v>20</v>
       </c>
@@ -2260,62 +2297,62 @@
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:18">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
         <v>21</v>
       </c>
       <c r="B23" s="8">
-        <v>0.1020294</v>
+        <v>0.10202940000000001</v>
       </c>
       <c r="C23" s="8">
-        <v>0.244517</v>
+        <v>0.24451700000000001</v>
       </c>
       <c r="E23" s="8">
-        <v>0.7455374</v>
+        <v>0.74553740000000002</v>
       </c>
       <c r="F23" s="8">
-        <v>0.0022118</v>
+        <v>2.2117999999999999E-3</v>
       </c>
       <c r="H23" s="8">
-        <v>0.1061302</v>
+        <v>0.10613019999999999</v>
       </c>
       <c r="I23" s="8">
-        <v>0.0581274</v>
+        <v>5.8127400000000003E-2</v>
       </c>
       <c r="K23" s="8">
-        <v>0.2748174</v>
+        <v>0.27481739999999999</v>
       </c>
       <c r="L23" s="8">
-        <v>0.0900606</v>
+        <v>9.0060600000000005E-2</v>
       </c>
       <c r="N23" s="8">
-        <v>0.0150892</v>
+        <v>1.5089200000000001E-2</v>
       </c>
       <c r="O23" s="8">
-        <v>0.3599654</v>
+        <v>0.35996539999999999</v>
       </c>
       <c r="Q23" s="8">
         <v>0.111458</v>
       </c>
       <c r="R23" s="8">
-        <v>0.2489166</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18">
+        <v>0.24891659999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
         <v>22</v>
       </c>
       <c r="B24" s="8">
-        <v>0.135868</v>
+        <v>0.13586799999999999</v>
       </c>
       <c r="C24" s="8">
-        <v>0.1304528</v>
+        <v>0.13045280000000001</v>
       </c>
       <c r="E24" s="8">
-        <v>0.0165828</v>
+        <v>1.6582800000000002E-2</v>
       </c>
       <c r="F24" s="8">
-        <v>0.0377314</v>
+        <v>3.7731399999999998E-2</v>
       </c>
       <c r="H24" s="8">
         <v>0.1816894</v>
@@ -2324,19 +2361,19 @@
         <v>0.1412014</v>
       </c>
       <c r="K24" s="8">
-        <v>0.1213758</v>
+        <v>0.12137580000000001</v>
       </c>
       <c r="L24" s="8">
-        <v>0.1326014</v>
+        <v>0.13260140000000001</v>
       </c>
       <c r="N24" s="8">
-        <v>0.1300194</v>
+        <v>0.13001940000000001</v>
       </c>
       <c r="O24" s="8">
-        <v>0.0887784</v>
+        <v>8.8778399999999993E-2</v>
       </c>
       <c r="Q24" s="8">
-        <v>0.1312598</v>
+        <v>0.13125980000000001</v>
       </c>
       <c r="R24" s="8">
         <v>0.1164258</v>

</xml_diff>